<commit_message>
All tables except fund are extracted and put in the db
</commit_message>
<xml_diff>
--- a/SampleModel.xlsx
+++ b/SampleModel.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12920" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12920" windowHeight="19540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -433,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -750,7 +751,7 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24">
-        <f t="shared" ref="B9:B24" si="2">MAX(I$2,(D24/8)^G$2)*(C23*(1+H$2))</f>
+        <f t="shared" ref="B24" si="2">MAX(I$2,(D24/8)^G$2)*(C23*(1+H$2))</f>
         <v>0</v>
       </c>
       <c r="C24">
@@ -770,4 +771,150 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>78</v>
+      </c>
+      <c r="D10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>89</v>
+      </c>
+      <c r="B11">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <v>95</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>